<commit_message>
Excel Reader and Data driven test has been added
</commit_message>
<xml_diff>
--- a/OnboardingTest2/OnboardingTest2/ExcelData/TestData.xlsx
+++ b/OnboardingTest2/OnboardingTest2/ExcelData/TestData.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27930" windowHeight="17180"/>
+    <workbookView windowWidth="19200" windowHeight="17780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
+    <sheet name="ManageListing" sheetId="3" r:id="rId2"/>
+    <sheet name="ShareSkill" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Emailaddress</t>
   </si>
@@ -22,21 +24,53 @@
     <t>Password</t>
   </si>
   <si>
-    <t>45107567@qq.com</t>
+    <t>451075672@qq.com</t>
   </si>
   <si>
     <t>abc123</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Deleteaction</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>SKTag</t>
+  </si>
+  <si>
+    <t>Jazz Club</t>
+  </si>
+  <si>
+    <t>We are true Jazz lover, If you are intrested in Jazz please feel free to join us!!</t>
+  </si>
+  <si>
+    <t>Photo Skill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="177" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -662,11 +696,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1022,8 +1065,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B$1:B$1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1032,20 +1075,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="10.6363636363636" customWidth="1"/>
+    <col min="2" max="2" width="92.8181818181818" customWidth="1"/>
+    <col min="3" max="3" width="17.3636363636364" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="6" width="11.8181818181818" customWidth="1"/>
+    <col min="7" max="8" width="10.6363636363636" customWidth="1"/>
+    <col min="10" max="10" width="16.2727272727273" customWidth="1"/>
+    <col min="11" max="11" width="21.9090909090909" customWidth="1"/>
+    <col min="12" max="12" width="7.54545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>